<commit_message>
Update progress tasks count and enumerate Planner plans for unified groups
</commit_message>
<xml_diff>
--- a/TenantAssessment-Template.xlsx
+++ b/TenantAssessment-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\AdminSeanMc\Tenant Migration Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TenantAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BED394-1DDD-45B7-808E-A9E12FCC34F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884E76E-DB9F-49E1-A46B-710905112828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-Level" sheetId="25" r:id="rId1"/>
@@ -480,35 +480,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,7 +812,7 @@
   <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,7 +907,7 @@
         <v>100</v>
       </c>
       <c r="B11" cm="1">
-        <f t="array" ref="B11">SUM((('SharePoint Sites'!I2:I1048576)/1024)/1024)/1024</f>
+        <f t="array" ref="B11">SUM((('SharePoint Sites'!J2:J1048576)/1024)/1024)/1024</f>
         <v>0</v>
       </c>
     </row>
@@ -950,7 +925,7 @@
         <v>97</v>
       </c>
       <c r="B13">
-        <f>SUM(Teams!D2:D1048576)</f>
+        <f>SUM(Teams!E2:E1048576)</f>
         <v>0</v>
       </c>
     </row>
@@ -959,7 +934,7 @@
         <v>111</v>
       </c>
       <c r="B14">
-        <f>SUM(Teams!E2:E1048576)</f>
+        <f>SUM(Teams!F2:F1048576)</f>
         <v>0</v>
       </c>
     </row>
@@ -968,7 +943,7 @@
         <v>112</v>
       </c>
       <c r="B15">
-        <f>SUM(Teams!I2:I1048576)</f>
+        <f>SUM(Teams!J2:J1048576)</f>
         <v>0</v>
       </c>
     </row>
@@ -977,7 +952,7 @@
         <v>101</v>
       </c>
       <c r="B16" cm="1">
-        <f t="array" ref="B16">ROUNDUP(SUM(((Teams!F2:F1048576)/1024)/1024)/1024,3)</f>
+        <f t="array" ref="B16">ROUNDUP(SUM(((Teams!G2:G1048576)/1024)/1024)/1024,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -986,7 +961,7 @@
         <v>102</v>
       </c>
       <c r="B17" cm="1">
-        <f t="array" ref="B17">ROUNDUP(SUM(((Teams!G2:G1048576)/1024)/1024)/1024,3)</f>
+        <f t="array" ref="B17">ROUNDUP(SUM(((Teams!H2:H1048576)/1024)/1024)/1024,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -995,7 +970,7 @@
         <v>113</v>
       </c>
       <c r="B18" cm="1">
-        <f t="array" ref="B18">ROUNDUP(SUM(((Teams!H2:H1048576)/1024)/1024)/1024,3)</f>
+        <f t="array" ref="B18">ROUNDUP(SUM(((Teams!I2:I1048576)/1024)/1024)/1024,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -1060,52 +1035,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1139,72 +1114,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="I2" s="14"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="I3" s="14"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="I4" s="14"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="I5" s="14"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="I6" s="14"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="I7" s="14"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="I8" s="14"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="I9" s="14"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="I10" s="14"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="I11" s="14"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="I12" s="14"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="I13" s="14"/>
+      <c r="I13" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J13" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
@@ -1236,63 +1211,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="I2" s="16"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="I4" s="16"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="I5" s="16"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="I7" s="16"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="I11" s="16"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="I13" s="16"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="I15" s="16"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="17" spans="9:9">
-      <c r="I17" s="16"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="20" spans="9:9">
-      <c r="I20" s="16"/>
+      <c r="I20" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J22" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
@@ -1318,25 +1293,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000011000000}"/>
@@ -1367,34 +1342,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1423,19 +1398,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1464,22 +1439,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1504,7 +1479,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="23"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000015000000}"/>
@@ -1527,7 +1502,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="24"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000016000000}"/>
@@ -1560,37 +1535,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1818,81 +1793,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="S2" s="3"/>
+      <c r="S2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -1937,99 +1912,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="S2" s="5"/>
+      <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:24">
-      <c r="S3" s="5"/>
+      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:24">
-      <c r="S4" s="5"/>
+      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="S5" s="5"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="S6" s="5"/>
+      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="S7" s="5"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="S8" s="5"/>
+      <c r="S8" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X8" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -2065,46 +2040,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2142,105 +2117,105 @@
     <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="27" customFormat="1">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="H2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="H2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="H3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="H3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="H4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="H4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="H5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="H5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="H6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="H6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="H7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="H7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="H8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="H8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="H9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="H9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="H10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="H10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="H11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="H11" s="1"/>
+      <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="H12" s="8"/>
-      <c r="N12" s="8"/>
+      <c r="H12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O12" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
@@ -2274,45 +2249,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="H2" s="9"/>
+      <c r="H2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -2338,16 +2313,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2374,9 +2349,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding missing columns and case of columns to work with PowerBI report
</commit_message>
<xml_diff>
--- a/TenantAssessment-Template.xlsx
+++ b/TenantAssessment-Template.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TenantAssessment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884E76E-DB9F-49E1-A46B-710905112828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92122E56-49D6-4819-954F-EBEF86705964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26985" yWindow="5070" windowWidth="23085" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-Level" sheetId="25" r:id="rId1"/>
@@ -42,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'MX Records'!$A$1:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'OneDrive Sites'!$A$1:$K$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Receive Connectors'!$A$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Resource Accounts'!$A$1:$X$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Resource Accounts'!$A$1:$Z$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Send Connectors'!$A$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Shared Mailboxes'!$A$1:$X$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SharePoint Sites'!$A$1:$N$44</definedName>
@@ -92,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="125">
   <si>
     <t>Migrate</t>
   </si>
@@ -437,13 +432,43 @@
   </si>
   <si>
     <t>Standard Groups</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>AccountEnabled</t>
+  </si>
+  <si>
+    <t>UserPrincipalName</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>GivenName</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Email Addresses</t>
+  </si>
+  <si>
+    <t>UsageLocation</t>
+  </si>
+  <si>
+    <t>UserType</t>
+  </si>
+  <si>
+    <t>OnPremisesSyncEnabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -458,6 +483,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -480,10 +511,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,9 +545,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -553,7 +585,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -659,7 +691,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -801,7 +833,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -815,14 +847,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -830,7 +862,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -839,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -848,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -857,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -866,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -875,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -884,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -893,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -902,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -911,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -920,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -929,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -938,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -947,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -956,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -965,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -974,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -983,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -992,15 +1024,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1014,7 +1047,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
@@ -1034,7 +1067,7 @@
     <col min="16" max="16" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1087,6 +1120,7 @@
   </sheetData>
   <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1099,7 +1133,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
@@ -1113,7 +1147,7 @@
     <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1145,45 +1179,46 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J13" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1196,7 +1231,7 @@
       <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
@@ -1210,7 +1245,7 @@
     <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1242,36 +1277,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I5" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I7" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I11" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
     </row>
-    <row r="17" spans="9:9">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
     </row>
-    <row r="20" spans="9:9">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J22" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1284,7 +1320,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -1292,7 +1328,7 @@
     <col min="5" max="5" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1309,13 +1345,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000011000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1328,7 +1365,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="3" width="41.7109375" customWidth="1"/>
@@ -1341,7 +1378,7 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
@@ -1376,6 +1413,7 @@
   </sheetData>
   <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0000-000012000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1388,7 +1426,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -1397,7 +1435,7 @@
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -1417,6 +1455,7 @@
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000013000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1429,7 +1468,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="9.140625" customWidth="1"/>
@@ -1438,7 +1477,7 @@
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -1461,6 +1500,7 @@
   </sheetData>
   <autoFilter ref="A1:F5" xr:uid="{00000000-0009-0000-0000-000014000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1473,17 +1513,18 @@
       <selection pane="bottomLeft" activeCell="D26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000015000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1496,17 +1537,18 @@
       <selection pane="bottomLeft" activeCell="D21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000016000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1519,7 +1561,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -1534,7 +1576,7 @@
     <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1572,6 +1614,7 @@
   </sheetData>
   <autoFilter ref="A1:K21" xr:uid="{00000000-0009-0000-0000-000017000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1584,7 +1627,7 @@
       <selection pane="bottomLeft" activeCell="I2" sqref="A2:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
@@ -1612,7 +1655,7 @@
     <col min="24" max="24" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1686,72 +1729,73 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S5" s="1"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S8" s="1"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S11" s="1"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S13" s="1"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="19:19">
+    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="19:19">
+    <row r="18" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="19:19">
+    <row r="19" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="19:19">
+    <row r="20" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="19:19">
+    <row r="21" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="19:19">
+    <row r="22" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S22" s="1"/>
     </row>
-    <row r="24" spans="19:19">
+    <row r="24" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="19:19">
+    <row r="25" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S25" s="1"/>
     </row>
-    <row r="27" spans="19:19">
+    <row r="27" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="19:19">
+    <row r="28" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="19:19">
+    <row r="29" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S29" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1764,7 +1808,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -1792,7 +1836,7 @@
     <col min="24" max="24" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1866,25 +1910,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1048542" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" customWidth="1"/>
@@ -1911,104 +1956,111 @@
     <col min="24" max="24" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="X1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S8" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X8" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:Z1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2021,7 +2073,7 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -2039,7 +2091,7 @@
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2086,6 +2138,7 @@
   </sheetData>
   <autoFilter ref="A1:N44" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2098,7 +2151,7 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
@@ -2117,7 +2170,7 @@
     <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2173,53 +2226,54 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H12" s="1"/>
       <c r="N12" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O12" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2232,7 +2286,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -2248,7 +2302,7 @@
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2286,12 +2340,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H2" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2304,7 +2359,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -2312,7 +2367,7 @@
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -2329,6 +2384,7 @@
   </sheetData>
   <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2341,19 +2397,20 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="A1:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" customWidth="1"/>
     <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>